<commit_message>
Added clear_page for SRS and ART to emforce cleearing of timeout
</commit_message>
<xml_diff>
--- a/data_raw/dicts/GEN_dict.xlsx
+++ b/data_raw/dicts/GEN_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171E55E0-B702-4DE0-A73B-7E849514E0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F58575-3806-4D72-BFE2-F1E3E503AC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
   <si>
     <t>key</t>
   </si>
@@ -323,6 +323,15 @@
   </si>
   <si>
     <t>Now the test starts.&lt;br&gt; Have fun!</t>
+  </si>
+  <si>
+    <t>YOU_FINISHED</t>
+  </si>
+  <si>
+    <t>Sie haben den {{test_name}} beendet.</t>
+  </si>
+  <si>
+    <t>You finished the {{test_name}}.</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,6 +1568,17 @@
         <v>100</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>